<commit_message>
Hydro implemented and tested
Tested with 1N. Should work for any case
</commit_message>
<xml_diff>
--- a/data/parameters_smspp.xlsx
+++ b/data/parameters_smspp.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -346,34 +346,31 @@
     <t>LineSusceptance</t>
   </si>
   <si>
+    <t>[NA]</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>[L]</t>
+  </si>
+  <si>
+    <t>1| [T][1]</t>
+  </si>
+  <si>
+    <t>[T][1]</t>
+  </si>
+  <si>
+    <t>[NR][T]</t>
+  </si>
+  <si>
     <t>[1][NR] | [T][NR]</t>
   </si>
   <si>
-    <t>[T][NR]</t>
-  </si>
-  <si>
-    <t>[NA]</t>
-  </si>
-  <si>
-    <t>[1][NA] | [T][NA]</t>
-  </si>
-  <si>
-    <t>[T][NA]</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>[L]</t>
-  </si>
-  <si>
-    <t>1| [T][1]</t>
-  </si>
-  <si>
-    <t>[T][1]</t>
+    <t>[NA] | [T][NA]</t>
   </si>
 </sst>
 </file>
@@ -743,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -763,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -783,10 +780,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -803,10 +800,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
@@ -823,10 +820,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -890,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -910,7 +907,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -930,7 +927,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -950,10 +947,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>9</v>
@@ -970,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>9</v>
@@ -990,10 +987,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -1010,10 +1007,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -1030,10 +1027,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
@@ -1050,10 +1047,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>9</v>
@@ -1070,10 +1067,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>9</v>
@@ -1090,10 +1087,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>9</v>
@@ -1110,10 +1107,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>9</v>
@@ -1130,10 +1127,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>9</v>
@@ -1150,10 +1147,10 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>9</v>
@@ -1170,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1190,10 +1187,10 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>9</v>
@@ -1210,10 +1207,10 @@
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>9</v>
@@ -1272,7 +1269,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1292,10 +1289,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -1312,10 +1309,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1332,10 +1329,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
@@ -1352,10 +1349,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -1372,10 +1369,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -1392,10 +1389,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -1412,10 +1409,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -1433,10 +1430,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -1453,10 +1450,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>14</v>
@@ -1473,10 +1470,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -1493,10 +1490,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -1513,7 +1510,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1536,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1559,10 +1556,10 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
@@ -1577,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,7 +1619,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1642,7 +1639,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1662,10 +1659,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1682,10 +1679,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
@@ -1702,10 +1699,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -1722,10 +1719,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -1742,10 +1739,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -1762,10 +1759,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -1782,10 +1779,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -1802,10 +1799,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
@@ -1822,10 +1819,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -1842,10 +1839,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -1862,10 +1859,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1882,10 +1879,10 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>14</v>
@@ -1902,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>89</v>
@@ -1922,7 +1919,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>89</v>
@@ -1942,10 +1939,10 @@
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -1962,10 +1959,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -1982,10 +1979,10 @@
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -2002,10 +1999,10 @@
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -2022,10 +2019,10 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2042,10 +2039,10 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>9</v>
@@ -2062,10 +2059,10 @@
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>14</v>
@@ -2121,10 +2118,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -2141,10 +2138,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -2161,10 +2158,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -2181,10 +2178,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
@@ -2201,10 +2198,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
@@ -2256,10 +2253,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -2276,10 +2273,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -2296,10 +2293,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -2316,10 +2313,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
@@ -2336,10 +2333,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>

</xml_diff>